<commit_message>
minor tweaks - v1.0
</commit_message>
<xml_diff>
--- a/ingredients.xlsx
+++ b/ingredients.xlsx
@@ -561,8 +561,8 @@
       <c r="K3" s="4">
         <v>8.5</v>
       </c>
-      <c r="L3" s="4">
-        <v>88.5</v>
+      <c r="L3" s="5">
+        <v>88.0</v>
       </c>
       <c r="M3" s="5">
         <v>100.0</v>

</xml_diff>

<commit_message>
added more ingredients, minor tweaks
</commit_message>
<xml_diff>
--- a/ingredients.xlsx
+++ b/ingredients.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Ingredient</t>
   </si>
@@ -93,7 +93,7 @@
     <t>Chocolate</t>
   </si>
   <si>
-    <t>Amul Dark Chocolate Sugar Free</t>
+    <t>Amul Dark Chocolate 55% Sugar Free</t>
   </si>
   <si>
     <t>Sugar</t>
@@ -102,18 +102,21 @@
     <t>Popular Essentials Refined Sugar</t>
   </si>
   <si>
+    <t>Thickener</t>
+  </si>
+  <si>
+    <t>Weikfield Cornstarch</t>
+  </si>
+  <si>
+    <t>Emulsifier</t>
+  </si>
+  <si>
+    <t>Meron Soy Lecithin</t>
+  </si>
+  <si>
     <t>Stabilizer</t>
   </si>
   <si>
-    <t>Weikfield Cornstarch</t>
-  </si>
-  <si>
-    <t>Emulsifier</t>
-  </si>
-  <si>
-    <t>Meron Soy Lecithin</t>
-  </si>
-  <si>
     <t>Meron Guar Gum</t>
   </si>
   <si>
@@ -124,6 +127,18 @@
   </si>
   <si>
     <t>Sid's Farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amul Dark Chocolate 75% </t>
+  </si>
+  <si>
+    <t>Amul Belgian Chocolate</t>
+  </si>
+  <si>
+    <t>Cocoa Powder</t>
+  </si>
+  <si>
+    <t>Hershey's Cocoa Powder</t>
   </si>
 </sst>
 </file>
@@ -177,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -196,10 +211,22 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -418,7 +445,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="29.29"/>
+    <col customWidth="1" min="1" max="1" width="29.29"/>
+    <col customWidth="1" min="2" max="2" width="33.14"/>
     <col customWidth="1" min="3" max="3" width="12.29"/>
     <col customWidth="1" min="4" max="4" width="10.29"/>
     <col customWidth="1" min="5" max="5" width="16.57"/>
@@ -766,7 +794,7 @@
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="4">
@@ -952,10 +980,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4">
         <v>208.0</v>
@@ -999,10 +1027,10 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="4">
         <v>387.0</v>
@@ -1045,11 +1073,11 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>35</v>
+      <c r="B14" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="C14" s="5">
         <v>64.7</v>
@@ -1090,6 +1118,152 @@
       </c>
       <c r="O14" s="5">
         <v>8.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="5">
+        <v>538.0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>9.6</v>
+      </c>
+      <c r="E15" s="5">
+        <v>37.4</v>
+      </c>
+      <c r="F15" s="5">
+        <v>25.3</v>
+      </c>
+      <c r="G15" s="5">
+        <v>39.8</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>57.0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="9">
+        <f>0.9*((24.5*100)+(0*100)+(0.8*190))/25.3</f>
+        <v>92.56126482</v>
+      </c>
+      <c r="N15" s="9">
+        <f>0.95*((24.5*100)+(0*16)+(0.8*130))/25.3</f>
+        <v>95.90118577</v>
+      </c>
+      <c r="O15" s="4">
+        <v>120.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="5">
+        <v>551.0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>8.7</v>
+      </c>
+      <c r="E16" s="5">
+        <v>51.2</v>
+      </c>
+      <c r="F16" s="5">
+        <v>49.6</v>
+      </c>
+      <c r="G16" s="5">
+        <v>35.3</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>155.0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="K16" s="10">
+        <f>1.07*(0.88*D16+8)</f>
+        <v>16.75192</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="M16" s="9">
+        <f>0.9*((40*100)+(8*100) + (1.6*190))/49.6</f>
+        <v>92.61290323</v>
+      </c>
+      <c r="N16" s="11">
+        <f>0.95*((40*100)+(8*16)+(1.6*130))/49.6</f>
+        <v>83.0483871</v>
+      </c>
+      <c r="O16" s="5">
+        <v>128.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="5">
+        <v>409.0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>19.6</v>
+      </c>
+      <c r="E17" s="5">
+        <v>58.0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="G17" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="M17" s="9">
+        <v>190.0</v>
+      </c>
+      <c r="N17" s="11">
+        <v>125.0</v>
+      </c>
+      <c r="O17" s="5">
+        <v>200.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
added more ingredients, total cost bugfix
</commit_message>
<xml_diff>
--- a/ingredients.xlsx
+++ b/ingredients.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>Ingredient</t>
   </si>
@@ -102,7 +102,7 @@
     <t>Popular Essentials Refined Sugar</t>
   </si>
   <si>
-    <t>Thickener</t>
+    <t>Stabilizer</t>
   </si>
   <si>
     <t>Weikfield Cornstarch</t>
@@ -114,9 +114,6 @@
     <t>Meron Soy Lecithin</t>
   </si>
   <si>
-    <t>Stabilizer</t>
-  </si>
-  <si>
     <t>Meron Guar Gum</t>
   </si>
   <si>
@@ -139,13 +136,22 @@
   </si>
   <si>
     <t>Hershey's Cocoa Powder</t>
+  </si>
+  <si>
+    <t>BAR70 Dark Couverture</t>
+  </si>
+  <si>
+    <t>BAR38 Milk Couverture</t>
+  </si>
+  <si>
+    <t>BAR Cocoa Powder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -162,6 +168,17 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -228,6 +245,27 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -980,10 +1018,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="C12" s="4">
         <v>208.0</v>
@@ -1027,10 +1065,10 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C13" s="4">
         <v>387.0</v>
@@ -1077,7 +1115,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="5">
         <v>64.7</v>
@@ -1125,7 +1163,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="5">
         <v>538.0</v>
@@ -1158,12 +1196,12 @@
         <v>0.0</v>
       </c>
       <c r="M15" s="9">
-        <f>0.9*((24.5*100)+(0*100)+(0.8*190))/25.3</f>
-        <v>92.56126482</v>
+        <f>((24.5*100)+(0*100)+(0.8*190))/25.3</f>
+        <v>102.8458498</v>
       </c>
       <c r="N15" s="9">
-        <f>0.95*((24.5*100)+(0*16)+(0.8*130))/25.3</f>
-        <v>95.90118577</v>
+        <f>((24.5*100)+(0*16)+(0.8*130))/25.3</f>
+        <v>100.9486166</v>
       </c>
       <c r="O15" s="4">
         <v>120.0</v>
@@ -1174,7 +1212,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="5">
         <v>551.0</v>
@@ -1208,12 +1246,12 @@
         <v>0.0</v>
       </c>
       <c r="M16" s="9">
-        <f>0.9*((40*100)+(8*100) + (1.6*190))/49.6</f>
-        <v>92.61290323</v>
+        <f>((40*100)+(8*100) + (1.6*190))/49.6</f>
+        <v>102.9032258</v>
       </c>
       <c r="N16" s="11">
-        <f>0.95*((40*100)+(8*16)+(1.6*130))/49.6</f>
-        <v>83.0483871</v>
+        <f>((40*100)+(8*16)+(1.6*130))/49.6</f>
+        <v>87.41935484</v>
       </c>
       <c r="O16" s="5">
         <v>128.0</v>
@@ -1221,10 +1259,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="C17" s="5">
         <v>409.0</v>
@@ -1257,12 +1295,170 @@
         <v>0.0</v>
       </c>
       <c r="M17" s="9">
-        <v>190.0</v>
+        <v>0.0</v>
       </c>
       <c r="N17" s="11">
-        <v>125.0</v>
+        <v>0.0</v>
       </c>
       <c r="O17" s="5">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="5">
+        <v>587.0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>50.3</v>
+      </c>
+      <c r="F18" s="5">
+        <v>31.0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>39.7</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>34.0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="M18" s="9">
+        <v>100.0</v>
+      </c>
+      <c r="N18" s="9">
+        <v>100.0</v>
+      </c>
+      <c r="O18" s="5">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="14">
+        <v>560.0</v>
+      </c>
+      <c r="D19" s="14">
+        <v>4.2</v>
+      </c>
+      <c r="E19" s="14">
+        <v>56.0</v>
+      </c>
+      <c r="F19" s="14">
+        <v>47.0</v>
+      </c>
+      <c r="G19" s="14">
+        <v>35.0</v>
+      </c>
+      <c r="H19" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="I19" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="J19" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="K19" s="16">
+        <f>1.07*(0.88*D19+6)</f>
+        <v>10.37472</v>
+      </c>
+      <c r="L19" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="M19" s="16">
+        <f>((46*100)+(5*100))/51</f>
+        <v>100</v>
+      </c>
+      <c r="N19" s="17">
+        <f>((46*100)+(5*16))/51</f>
+        <v>91.76470588</v>
+      </c>
+      <c r="O19" s="14">
+        <v>145.0</v>
+      </c>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="18"/>
+      <c r="V19" s="18"/>
+      <c r="W19" s="18"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="18"/>
+      <c r="Z19" s="18"/>
+      <c r="AA19" s="18"/>
+      <c r="AB19" s="18"/>
+      <c r="AC19" s="18"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="5">
+        <v>313.0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="E20" s="5">
+        <v>45.7</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>25.0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="M20" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="N20" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="O20" s="5">
         <v>200.0</v>
       </c>
     </row>

</xml_diff>